<commit_message>
Updated input files and interface for additional ponding methods added nitrous oxide as a gas
</commit_message>
<xml_diff>
--- a/Example input/SoybeanInputs.xlsx
+++ b/Example input/SoybeanInputs.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1A58C6-BD7E-4016-88D5-DF496F9D7804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AC97DF-B364-4AE5-988F-9734A859D58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1725" yWindow="570" windowWidth="25920" windowHeight="13425" tabRatio="824" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2565" windowWidth="26475" windowHeight="11295" tabRatio="824" firstSheet="3" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="5" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="WaterMovParam" sheetId="22" r:id="rId17"/>
     <sheet name="MulchDecomp" sheetId="18" r:id="rId18"/>
     <sheet name="MulchGeo" sheetId="21" r:id="rId19"/>
+    <sheet name="Sheet1" sheetId="23" r:id="rId20"/>
   </sheets>
   <definedNames>
     <definedName name="GridX">#REF!</definedName>
@@ -1459,7 +1460,8 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+  <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{805AD1FC-2209-4009-A12C-354884B60DC8}"/>
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
@@ -1766,7 +1768,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -1787,6 +1789,7 @@
     <col min="14" max="14" width="14.140625" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -5478,8 +5481,8 @@
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5540,7 +5543,7 @@
         <v>-100000</v>
       </c>
       <c r="F2" s="8">
-        <v>10000000000</v>
+        <v>1E-3</v>
       </c>
       <c r="G2">
         <v>0.02</v>
@@ -5860,6 +5863,18 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97106E43-F276-44E7-8ECC-7DD6287E7810}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
@@ -6481,7 +6496,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -6638,6 +6653,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010086EABF47CD1113448A96A17F6C8D13F9" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="562d1dd5ad8dfb6d09dfa11834733c42">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a5f42ec3-4ee2-45fc-8d77-288bf2f0f986" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7128e87dc4ae7544fa3e3576daab8407" ns2:_="">
     <xsd:import namespace="a5f42ec3-4ee2-45fc-8d77-288bf2f0f986"/>
@@ -6801,22 +6831,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB355063-4085-408A-B581-F3B4C870A3FF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{532DCAAA-3F51-4B5E-8815-DDBB9D55C2DB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5088F4C1-76EA-4EB8-857C-42C0075C1F9C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6832,21 +6864,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{532DCAAA-3F51-4B5E-8815-DDBB9D55C2DB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB355063-4085-408A-B581-F3B4C870A3FF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>